<commit_message>
'actualización 03 01 2021'
</commit_message>
<xml_diff>
--- a/scrap_sanidad/datos_sanidad/clave_numero_fecha.xlsx
+++ b/scrap_sanidad/datos_sanidad/clave_numero_fecha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharias/Documents/proyectos/covid/scrap_sanidad/datos_sanidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCB2357-7166-ED4E-818B-D41ABBDE76EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22061BA9-4183-7A40-A4BE-101E4F886534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clave_numero_fecha" sheetId="1" r:id="rId1"/>
@@ -878,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2494,6 +2494,54 @@
         <v>44187</v>
       </c>
     </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>277</v>
+      </c>
+      <c r="B202" s="1">
+        <v>44188</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>278</v>
+      </c>
+      <c r="B203" s="1">
+        <v>44189</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>279</v>
+      </c>
+      <c r="B204" s="1">
+        <v>44193</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>280</v>
+      </c>
+      <c r="B205" s="1">
+        <v>44194</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>281</v>
+      </c>
+      <c r="B206" s="1">
+        <v>44195</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>282</v>
+      </c>
+      <c r="B207" s="1">
+        <v>44196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion vacunas 18 febrero
</commit_message>
<xml_diff>
--- a/scrap_sanidad/datos_sanidad/clave_numero_fecha.xlsx
+++ b/scrap_sanidad/datos_sanidad/clave_numero_fecha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharias/Documents/proyectos/covid/scrap_sanidad/datos_sanidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC4872B-3BDF-CD44-A7CA-062D1EB1A74F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641B683F-D972-7142-93E8-DC98720680BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B238"/>
+  <dimension ref="A1:B239"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2790,6 +2790,14 @@
         <v>44243</v>
       </c>
     </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>314</v>
+      </c>
+      <c r="B239" s="1">
+        <v>44244</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>